<commit_message>
avances en costos variables
</commit_message>
<xml_diff>
--- a/SAP - NEGOCIO/Temporal/Presupuesto/Borrador Costos.xlsx
+++ b/SAP - NEGOCIO/Temporal/Presupuesto/Borrador Costos.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Costos Fijos" sheetId="1" r:id="rId1"/>
     <sheet name="Costos Variables" sheetId="2" r:id="rId2"/>
-    <sheet name="Remuneraciones" sheetId="3" r:id="rId3"/>
-    <sheet name="Amortizaciones " sheetId="5" r:id="rId4"/>
-    <sheet name="Depreciaciones" sheetId="4" r:id="rId5"/>
-    <sheet name="Impuestos" sheetId="6" r:id="rId6"/>
+    <sheet name="Estimacion de pedidos" sheetId="7" r:id="rId3"/>
+    <sheet name="Remuneraciones" sheetId="3" r:id="rId4"/>
+    <sheet name="Amortizaciones " sheetId="5" r:id="rId5"/>
+    <sheet name="Depreciaciones" sheetId="4" r:id="rId6"/>
+    <sheet name="Impuestos" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="87">
   <si>
     <t>Hosting</t>
   </si>
@@ -60,9 +61,6 @@
     <t>Costos Administrativos</t>
   </si>
   <si>
-    <t>Acesoría Legal</t>
-  </si>
-  <si>
     <t>Seguros</t>
   </si>
   <si>
@@ -244,14 +242,58 @@
   </si>
   <si>
     <t>Asesoría Contable</t>
+  </si>
+  <si>
+    <t>??????</t>
+  </si>
+  <si>
+    <t>Inflación</t>
+  </si>
+  <si>
+    <t>???fijo o variable?</t>
+  </si>
+  <si>
+    <t>Consumo por km</t>
+  </si>
+  <si>
+    <t>Precio de combustible</t>
+  </si>
+  <si>
+    <t>Periodo</t>
+  </si>
+  <si>
+    <t>% estimado de pedidos</t>
+  </si>
+  <si>
+    <t>Estimado estandar de pedidos por semestre año 1</t>
+  </si>
+  <si>
+    <t>Estimado estandar de pedidos por semestre año 2</t>
+  </si>
+  <si>
+    <t>Medidas estimadas</t>
+  </si>
+  <si>
+    <t>Porcentajes estimados</t>
+  </si>
+  <si>
+    <t>Estimado Km por pedido en promedio</t>
+  </si>
+  <si>
+    <t>????????</t>
+  </si>
+  <si>
+    <t>Asesoría Legal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$$-2C0A]\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="[$$-2C0A]#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -277,7 +319,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -335,6 +377,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -405,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -415,10 +463,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -427,8 +473,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -458,6 +502,18 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -792,13 +848,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
@@ -809,26 +865,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="C1" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="E1" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="41" t="s">
+      <c r="F1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="39" t="s">
-        <v>23</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -844,453 +900,456 @@
       <c r="S1" s="4"/>
     </row>
     <row r="2" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="40">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="36">
         <v>14.79</v>
       </c>
-      <c r="G2" s="27">
+      <c r="G2" s="23">
         <v>0.2</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="43">
+      <c r="B3" s="39">
         <v>5088</v>
       </c>
-      <c r="C3" s="43">
+      <c r="C3" s="39">
         <f>B3+(B3*G2)</f>
         <v>6105.6</v>
       </c>
-      <c r="D3" s="44">
+      <c r="D3" s="40">
         <f>C3+(B3*G2)</f>
         <v>7123.2000000000007</v>
       </c>
-      <c r="E3" s="44">
+      <c r="E3" s="40">
         <f>D3+(B3*G2)</f>
         <v>8140.8000000000011</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="43">
+      <c r="A4" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="39">
         <f>SUM(Remuneraciones!I14,Remuneraciones!I17)*6</f>
         <v>444039</v>
       </c>
-      <c r="C4" s="43">
+      <c r="C4" s="39">
         <f>B4+$B$4*$G$2</f>
         <v>532846.80000000005</v>
       </c>
-      <c r="D4" s="44">
+      <c r="D4" s="40">
         <f t="shared" ref="D4:E4" si="0">C4+$B$4*$G$2</f>
         <v>621654.60000000009</v>
       </c>
-      <c r="E4" s="44">
+      <c r="E4" s="40">
         <f t="shared" si="0"/>
         <v>710462.40000000014</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="43">
+      <c r="A5" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="39">
         <f>SUM(Remuneraciones!I25)*6</f>
         <v>261573</v>
       </c>
-      <c r="C5" s="43">
+      <c r="C5" s="39">
         <f>B5+B5*G2</f>
         <v>313887.59999999998</v>
       </c>
-      <c r="D5" s="44">
+      <c r="D5" s="40">
         <f>C5*2+C5*2*G2</f>
         <v>753330.24</v>
       </c>
-      <c r="E5" s="44">
+      <c r="E5" s="40">
         <f>D5+D5*G2</f>
         <v>903996.28799999994</v>
       </c>
     </row>
     <row r="6" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="43">
+      <c r="B6" s="39">
         <f>770*6</f>
         <v>4620</v>
       </c>
-      <c r="C6" s="43">
+      <c r="C6" s="39">
         <f>B6+B6*G2</f>
         <v>5544</v>
       </c>
-      <c r="D6" s="44">
+      <c r="D6" s="40">
         <f>C6+$B$6*$G$2</f>
         <v>6468</v>
       </c>
-      <c r="E6" s="44">
+      <c r="E6" s="40">
         <f>D6+$B$6*$G$2</f>
         <v>7392</v>
       </c>
     </row>
     <row r="7" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="43">
+      <c r="B7" s="39">
         <v>972</v>
       </c>
-      <c r="C7" s="43">
+      <c r="C7" s="39">
         <f>B7+$B$7*$G$2</f>
         <v>1166.4000000000001</v>
       </c>
-      <c r="D7" s="44">
+      <c r="D7" s="40">
         <f t="shared" ref="D7:E7" si="1">C7+$B$7*$G$2</f>
         <v>1360.8000000000002</v>
       </c>
-      <c r="E7" s="44">
+      <c r="E7" s="40">
         <f t="shared" si="1"/>
         <v>1555.2000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="43">
+      <c r="B8" s="39">
         <f>(25*F2)*6</f>
         <v>2218.5</v>
       </c>
-      <c r="C8" s="43">
+      <c r="C8" s="39">
         <f>B8+$B$8*$G$2</f>
         <v>2662.2</v>
       </c>
-      <c r="D8" s="44">
+      <c r="D8" s="40">
         <f t="shared" ref="D8:E8" si="2">C8+$B$8*$G$2</f>
         <v>3105.8999999999996</v>
       </c>
-      <c r="E8" s="44">
+      <c r="E8" s="40">
         <f t="shared" si="2"/>
         <v>3549.5999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="36">
+    <row r="9" spans="1:19" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="32">
         <f>SUM(B3:B8)</f>
         <v>718510.5</v>
       </c>
-      <c r="C9" s="36">
+      <c r="C9" s="32">
         <f>SUM(C3:C8)</f>
         <v>862212.6</v>
       </c>
-      <c r="D9" s="36">
+      <c r="D9" s="32">
         <f>SUM(D3:D8)</f>
         <v>1393042.74</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="32">
         <f>SUM(E3:E8)</f>
         <v>1635096.2880000002</v>
       </c>
     </row>
     <row r="10" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
     </row>
     <row r="11" spans="1:19" s="3" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="43">
+      <c r="A11" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="39">
         <f>SUM(Remuneraciones!I5,Remuneraciones!I9,Remuneraciones!I19)*6</f>
         <v>617157</v>
       </c>
-      <c r="C11" s="43">
+      <c r="C11" s="39">
         <f>B11+$B$11*$G$2</f>
         <v>740588.4</v>
       </c>
-      <c r="D11" s="44">
+      <c r="D11" s="40">
         <f t="shared" ref="D11:E11" si="3">C11+$B$11*$G$2</f>
         <v>864019.8</v>
       </c>
-      <c r="E11" s="44">
+      <c r="E11" s="40">
         <f t="shared" si="3"/>
         <v>987451.20000000007</v>
       </c>
     </row>
     <row r="12" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="43">
+      <c r="A12" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="39">
         <f>(900*5*6)</f>
         <v>27000</v>
       </c>
-      <c r="C12" s="43">
+      <c r="C12" s="39">
         <f>B12+$B$12*$G$2</f>
         <v>32400</v>
       </c>
-      <c r="D12" s="44">
+      <c r="D12" s="40">
         <f t="shared" ref="D12:E12" si="4">C12+$B$12*$G$2</f>
         <v>37800</v>
       </c>
-      <c r="E12" s="44">
+      <c r="E12" s="40">
         <f t="shared" si="4"/>
         <v>43200</v>
       </c>
     </row>
     <row r="13" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="43">
+      <c r="B13" s="39">
         <f>300*5*6</f>
         <v>9000</v>
       </c>
-      <c r="C13" s="43">
+      <c r="C13" s="39">
         <f>B13+$B$13*$G$2</f>
         <v>10800</v>
       </c>
-      <c r="D13" s="44">
+      <c r="D13" s="40">
         <f t="shared" ref="D13:E13" si="5">C13+$B$13*$G$2</f>
         <v>12600</v>
       </c>
-      <c r="E13" s="44">
+      <c r="E13" s="40">
         <f t="shared" si="5"/>
         <v>14400</v>
       </c>
     </row>
     <row r="14" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="43">
+      <c r="A14" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="39">
         <f>6200*6</f>
         <v>37200</v>
       </c>
-      <c r="C14" s="43">
+      <c r="C14" s="39">
         <f>B14+$B$14*$G$2</f>
         <v>44640</v>
       </c>
-      <c r="D14" s="44">
+      <c r="D14" s="40">
         <f t="shared" ref="D14:E14" si="6">C14+$B$14*$G$2</f>
         <v>52080</v>
       </c>
-      <c r="E14" s="44">
+      <c r="E14" s="40">
         <f t="shared" si="6"/>
         <v>59520</v>
       </c>
     </row>
     <row r="15" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="43">
+      <c r="A15" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="39">
         <f>380*6</f>
         <v>2280</v>
       </c>
-      <c r="C15" s="43">
+      <c r="C15" s="39">
         <f>B15+$B$15*G2</f>
         <v>2736</v>
       </c>
-      <c r="D15" s="44">
+      <c r="D15" s="40">
         <f t="shared" ref="D15:E15" si="7">C15+$B$15*H2</f>
         <v>2736</v>
       </c>
-      <c r="E15" s="44">
+      <c r="E15" s="40">
         <f t="shared" si="7"/>
         <v>2736</v>
       </c>
+      <c r="F15" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="16" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="43">
+      <c r="A16" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="39">
         <f>59.9*6</f>
         <v>359.4</v>
       </c>
-      <c r="C16" s="43">
+      <c r="C16" s="39">
         <f>B16+$B$16*G2</f>
         <v>431.28</v>
       </c>
-      <c r="D16" s="44">
+      <c r="D16" s="40">
         <f t="shared" ref="D16:E16" si="8">C16+$B$16*H2</f>
         <v>431.28</v>
       </c>
-      <c r="E16" s="44">
+      <c r="E16" s="40">
         <f t="shared" si="8"/>
         <v>431.28</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="B17" s="43"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-    </row>
-    <row r="18" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="36">
+      <c r="A17" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+    </row>
+    <row r="18" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="32">
         <f>SUM(B11:B17)</f>
         <v>692996.4</v>
       </c>
-      <c r="C18" s="36">
+      <c r="C18" s="32">
         <f>SUM(C11:C17)</f>
         <v>831595.68</v>
       </c>
-      <c r="D18" s="36">
+      <c r="D18" s="32">
         <f>SUM(D11:D17)</f>
         <v>969667.08000000007</v>
       </c>
-      <c r="E18" s="36">
+      <c r="E18" s="32">
         <f>SUM(E11:E17)</f>
         <v>1107738.4800000002</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
+      <c r="A19" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
     </row>
     <row r="20" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="B20" s="43">
+      <c r="A20" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="39">
         <v>12000</v>
       </c>
-      <c r="C20" s="43">
+      <c r="C20" s="39">
         <f>B20+$B$20*$G$2</f>
         <v>14400</v>
       </c>
-      <c r="D20" s="44">
+      <c r="D20" s="40">
         <f t="shared" ref="D20:E20" si="9">C20+$B$20*$G$2</f>
         <v>16800</v>
       </c>
-      <c r="E20" s="44">
+      <c r="E20" s="40">
         <f t="shared" si="9"/>
         <v>19200</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" s="43">
+      <c r="A21" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="39">
         <f>3000*6</f>
         <v>18000</v>
       </c>
-      <c r="C21" s="43">
+      <c r="C21" s="39">
         <f>B21+$B$21*$G$2</f>
         <v>21600</v>
       </c>
-      <c r="D21" s="44">
+      <c r="D21" s="40">
         <f t="shared" ref="D21:E21" si="10">C21+$B$21*$G$2</f>
         <v>25200</v>
       </c>
-      <c r="E21" s="44">
+      <c r="E21" s="40">
         <f t="shared" si="10"/>
         <v>28800</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="43">
+      <c r="A22" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="39">
         <v>4650</v>
       </c>
-      <c r="C22" s="43"/>
-      <c r="D22" s="44">
+      <c r="C22" s="39"/>
+      <c r="D22" s="40">
         <f>B22+B22*(G2*2)</f>
         <v>6510</v>
       </c>
-      <c r="E22" s="44"/>
-    </row>
-    <row r="23" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="36">
+      <c r="E22" s="40"/>
+    </row>
+    <row r="23" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="32">
         <f>SUM(B20:B22)</f>
         <v>34650</v>
       </c>
-      <c r="C23" s="36">
+      <c r="C23" s="32">
         <f>SUM(C20:C22)</f>
         <v>36000</v>
       </c>
-      <c r="D23" s="36">
+      <c r="D23" s="32">
         <f>SUM(D20:D22)</f>
         <v>48510</v>
       </c>
-      <c r="E23" s="36">
+      <c r="E23" s="32">
         <f>SUM(E20:E22)</f>
         <v>48000</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="38">
+    <row r="24" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="34">
         <f>SUM(B23,B18,B9)</f>
         <v>1446156.9</v>
       </c>
-      <c r="C24" s="38">
+      <c r="C24" s="34">
         <f>SUM(C23,C18,C9)</f>
         <v>1729808.28</v>
       </c>
-      <c r="D24" s="38">
+      <c r="D24" s="34">
         <f>SUM(D23,D18,D9)</f>
         <v>2411219.8200000003</v>
       </c>
-      <c r="E24" s="38">
+      <c r="E24" s="34">
         <f>SUM(E23,E18,E9)</f>
         <v>2790834.7680000002</v>
       </c>
-      <c r="F24" s="33"/>
-      <c r="G24" s="34">
+      <c r="F24" s="29"/>
+      <c r="G24" s="30">
         <f>SUM(B24:F24)</f>
         <v>8378019.7680000002</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="47">
+      <c r="B26" s="43">
         <f>SUM(C24,B24)</f>
         <v>3175965.1799999997</v>
       </c>
-      <c r="D26" s="47">
+      <c r="D26" s="43">
         <f>SUM(D24,E24)</f>
         <v>5202054.5880000005</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="47"/>
+      <c r="B28" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1300,16 +1359,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S15"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" customWidth="1"/>
@@ -1318,24 +1377,26 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="4"/>
+      <c r="G1" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -1357,136 +1418,315 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
-      <c r="F2" s="23"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="51">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="3" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="24"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46">
+        <f>3980+3980*G2</f>
+        <v>4776</v>
+      </c>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47">
+        <f>3980+3980*60%</f>
+        <v>6368</v>
+      </c>
+      <c r="F3" s="20"/>
     </row>
     <row r="4" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="24"/>
+        <v>68</v>
+      </c>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="47">
+        <f>99500+99500*40%</f>
+        <v>139300</v>
+      </c>
+      <c r="E4" s="48"/>
+      <c r="F4" s="20"/>
     </row>
     <row r="5" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="24"/>
+        <v>64</v>
+      </c>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="20" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="6" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="24"/>
+      <c r="B6" s="46">
+        <f>('Estimacion de pedidos'!B4+'Estimacion de pedidos'!B4*'Estimacion de pedidos'!B11)*'Estimacion de pedidos'!B3*'Estimacion de pedidos'!B2*'Estimacion de pedidos'!B6</f>
+        <v>73664.639999999999</v>
+      </c>
+      <c r="C6" s="46">
+        <f>('Estimacion de pedidos'!B4+'Estimacion de pedidos'!B4*'Estimacion de pedidos'!B12)*'Estimacion de pedidos'!B3*'Estimacion de pedidos'!B2*'Estimacion de pedidos'!B6+B6*G2</f>
+        <v>96582.528000000006</v>
+      </c>
+      <c r="D6" s="47">
+        <f>('Estimacion de pedidos'!B5+'Estimacion de pedidos'!B5*'Estimacion de pedidos'!B13)*'Estimacion de pedidos'!B3*'Estimacion de pedidos'!B2*'Estimacion de pedidos'!B6+C6*G2</f>
+        <v>167055.0336</v>
+      </c>
+      <c r="E6" s="48">
+        <f>('Estimacion de pedidos'!B5+'Estimacion de pedidos'!B5*'Estimacion de pedidos'!B14)*'Estimacion de pedidos'!B3*'Estimacion de pedidos'!B2*'Estimacion de pedidos'!B6+D6*G2</f>
+        <v>188925.24672</v>
+      </c>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="24"/>
-    </row>
-    <row r="8" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="B7" s="46">
+        <f>C7+C7*'Estimacion de pedidos'!B11</f>
+        <v>540</v>
+      </c>
+      <c r="C7" s="46">
+        <f>500+500*G2</f>
+        <v>600</v>
+      </c>
+      <c r="D7" s="47">
+        <f>(C7+C7*'Estimacion de pedidos'!B13)+C7*G2</f>
+        <v>690</v>
+      </c>
+      <c r="E7" s="47">
+        <f>(D7+D7*'Estimacion de pedidos'!B14)+D7*G2</f>
+        <v>828</v>
+      </c>
+      <c r="F7" s="20"/>
+    </row>
+    <row r="8" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="46">
+        <f>SUM(B6:B7)</f>
+        <v>74204.639999999999</v>
+      </c>
+      <c r="C8" s="46">
+        <f>SUM(C3:C7)</f>
+        <v>101958.52800000001</v>
+      </c>
+      <c r="D8" s="47">
+        <f>SUM(D3:D7)</f>
+        <v>307045.03359999997</v>
+      </c>
+      <c r="E8" s="48">
+        <f>SUM(E3:E7)</f>
+        <v>196121.24672</v>
+      </c>
+      <c r="F8" s="20"/>
+    </row>
+    <row r="9" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="25"/>
-    </row>
-    <row r="9" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="24"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
+        <v>7</v>
+      </c>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="20" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="11" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="24"/>
-    </row>
-    <row r="12" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+    </row>
+    <row r="12" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="25"/>
-    </row>
-    <row r="13" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="24"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="20"/>
+    </row>
+    <row r="13" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="24"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="F15" s="26"/>
+        <v>15</v>
+      </c>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="20"/>
+    </row>
+    <row r="15" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="46"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="20"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F16" s="22"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="52"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="53">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="53">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="53">
+        <v>25200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="53">
+        <f>B4+B4*90%</f>
+        <v>47880</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="54">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="52"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="53" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="55">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="55">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="55">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A9:B9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD28"/>
   <sheetViews>
@@ -1508,34 +1748,34 @@
   <sheetData>
     <row r="1" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="E1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>48</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:9 16384:16384" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -1546,61 +1786,61 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9 16384:16384" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="13">
+    <row r="3" spans="1:9 16384:16384" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="11">
         <v>24000</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13">
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11">
         <f>SUM(B3:D3)</f>
         <v>24000</v>
       </c>
     </row>
-    <row r="4" spans="1:9 16384:16384" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="13">
+    <row r="4" spans="1:9 16384:16384" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="11">
         <v>24000</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13">
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11">
         <f>SUM(B4:D4)</f>
         <v>24000</v>
       </c>
     </row>
-    <row r="5" spans="1:9 16384:16384" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16">
+    <row r="5" spans="1:9 16384:16384" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14">
         <f>SUM(I3:I4)</f>
         <v>48000</v>
       </c>
     </row>
     <row r="6" spans="1:9 16384:16384" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1611,61 +1851,61 @@
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="1:9 16384:16384" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="13">
+    <row r="7" spans="1:9 16384:16384" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="11">
         <v>20000</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13">
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11">
         <f>SUM(B7:D7)</f>
         <v>20000</v>
       </c>
     </row>
-    <row r="8" spans="1:9 16384:16384" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="13">
+    <row r="8" spans="1:9 16384:16384" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="11">
         <v>10907</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13">
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11">
         <f>SUM(B8:G8)</f>
         <v>10907</v>
       </c>
     </row>
-    <row r="9" spans="1:9 16384:16384" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16">
+    <row r="9" spans="1:9 16384:16384" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14">
         <f>SUM(I7:I8)</f>
         <v>30907</v>
       </c>
     </row>
     <row r="10" spans="1:9 16384:16384" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1676,89 +1916,89 @@
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9 16384:16384" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="13">
+    <row r="11" spans="1:9 16384:16384" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="11">
         <v>18425</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="11">
         <v>5527.5</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13">
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11">
         <f>SUM(B11:G11)</f>
         <v>23952.5</v>
       </c>
     </row>
-    <row r="12" spans="1:9 16384:16384" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="13">
+    <row r="12" spans="1:9 16384:16384" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="11">
         <v>15125</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="11">
         <v>2420</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13">
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11">
         <f>SUM(B12:G12)</f>
         <v>17545</v>
       </c>
     </row>
-    <row r="13" spans="1:9 16384:16384" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="13">
+    <row r="13" spans="1:9 16384:16384" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="11">
         <v>15125</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="11">
         <v>2420</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13">
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11">
         <f>SUM(B13,C13)</f>
         <v>17545</v>
       </c>
-      <c r="XFD13" s="15">
+      <c r="XFD13" s="13">
         <f>SUM(B13:XFC13)</f>
         <v>35090</v>
       </c>
     </row>
-    <row r="14" spans="1:9 16384:16384" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16">
+    <row r="14" spans="1:9 16384:16384" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14">
         <f>SUM(I11:I13)</f>
         <v>59042.5</v>
       </c>
     </row>
     <row r="15" spans="1:9 16384:16384" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -1769,45 +2009,45 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9 16384:16384" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="13">
+    <row r="16" spans="1:9 16384:16384" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="11">
         <v>12900</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="11">
         <v>2064</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13">
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11">
         <f>SUM(B16:G16)</f>
         <v>14964</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16">
+    <row r="17" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14">
         <f>SUM(I16)</f>
         <v>14964</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -1818,189 +2058,189 @@
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="13">
+    <row r="19" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="11">
         <v>18425</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="11">
         <v>5527.5</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13">
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11">
         <f>SUM(B19:H19)</f>
         <v>23952.5</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="13">
+    <row r="20" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="11">
         <v>7824</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="11">
         <v>2670</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13">
+      <c r="D20" s="11"/>
+      <c r="E20" s="11">
         <v>-1274.9000000000001</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="11">
         <v>-273</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="11">
         <v>-227</v>
       </c>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13">
+      <c r="H20" s="11"/>
+      <c r="I20" s="11">
         <f>SUM(E20:G20,C20,B20)</f>
         <v>8719.1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="13">
+    <row r="21" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="11">
         <v>7824</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="11">
         <v>2670</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13">
+      <c r="D21" s="11"/>
+      <c r="E21" s="11">
         <v>-1274.9000000000001</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="11">
         <v>-273</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="11">
         <v>-227</v>
       </c>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13">
+      <c r="H21" s="11"/>
+      <c r="I21" s="11">
         <f>SUM(E21:G21,C21,B21)</f>
         <v>8719.1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="13">
+    <row r="22" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="11">
         <v>7824</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="11">
         <v>2670</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13">
+      <c r="D22" s="11"/>
+      <c r="E22" s="11">
         <v>-1274.9000000000001</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="11">
         <v>-273</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="11">
         <v>-227</v>
       </c>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13">
+      <c r="H22" s="11"/>
+      <c r="I22" s="11">
         <f>SUM(E22:G22,C22,B22)</f>
         <v>8719.1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="13">
+    <row r="23" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="11">
         <v>7824</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="11">
         <v>2670</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13">
+      <c r="D23" s="11"/>
+      <c r="E23" s="11">
         <v>-1274.9000000000001</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F23" s="11">
         <v>-273</v>
       </c>
-      <c r="G23" s="13">
+      <c r="G23" s="11">
         <v>-227</v>
       </c>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13">
+      <c r="H23" s="11"/>
+      <c r="I23" s="11">
         <f>SUM(E23:G23,C23,B23)</f>
         <v>8719.1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="13">
+    <row r="24" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="11">
         <v>7824</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="11">
         <v>2670</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13">
+      <c r="D24" s="11"/>
+      <c r="E24" s="11">
         <v>-1274.9000000000001</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24" s="11">
         <v>-273</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G24" s="11">
         <v>-227</v>
       </c>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13">
+      <c r="H24" s="11"/>
+      <c r="I24" s="11">
         <f>SUM(E24:G24,C24,B24)</f>
         <v>8719.1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="19">
+    <row r="25" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="17">
         <f>SUM(I20:I24)</f>
         <v>43595.5</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I26" s="20">
+        <v>43</v>
+      </c>
+      <c r="I26" s="18">
         <f>SUM(I25,I17,I14,I9,I5)</f>
         <v>196509</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
+      <c r="A28" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2010,7 +2250,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
@@ -2028,16 +2268,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -2045,138 +2285,297 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-    </row>
-    <row r="3" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-    </row>
-    <row r="4" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-    </row>
-    <row r="5" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-    </row>
-    <row r="6" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-    </row>
-    <row r="7" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-    </row>
-    <row r="8" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-    </row>
-    <row r="9" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-    </row>
-    <row r="10" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-    </row>
-    <row r="11" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-    </row>
-    <row r="12" spans="1:9" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
+    <row r="2" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+    </row>
+    <row r="3" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+    </row>
+    <row r="4" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+    </row>
+    <row r="5" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+    </row>
+    <row r="6" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+    </row>
+    <row r="7" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+    </row>
+    <row r="8" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+    </row>
+    <row r="9" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+    </row>
+    <row r="10" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+    </row>
+    <row r="11" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+    </row>
+    <row r="12" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2190,166 +2589,7 @@
         <v>62</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -2360,125 +2600,125 @@
       <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Agregado Costos legales + algunos conceptos de inversión inicial
</commit_message>
<xml_diff>
--- a/SAP - NEGOCIO/Temporal/Presupuesto/Borrador Costos.xlsx
+++ b/SAP - NEGOCIO/Temporal/Presupuesto/Borrador Costos.xlsx
@@ -9,12 +9,16 @@
   <sheets>
     <sheet name="Costos Fijos" sheetId="1" r:id="rId1"/>
     <sheet name="Costos Variables" sheetId="2" r:id="rId2"/>
-    <sheet name="Estimacion de pedidos" sheetId="7" r:id="rId3"/>
-    <sheet name="Remuneraciones" sheetId="3" r:id="rId4"/>
-    <sheet name="Amortizaciones " sheetId="5" r:id="rId5"/>
-    <sheet name="Depreciaciones" sheetId="4" r:id="rId6"/>
-    <sheet name="Impuestos" sheetId="6" r:id="rId7"/>
+    <sheet name="Costos legales" sheetId="8" r:id="rId3"/>
+    <sheet name="Estimacion de pedidos" sheetId="7" r:id="rId4"/>
+    <sheet name="Remuneraciones" sheetId="3" r:id="rId5"/>
+    <sheet name="Amortizaciones " sheetId="5" r:id="rId6"/>
+    <sheet name="Depreciaciones" sheetId="4" r:id="rId7"/>
+    <sheet name="Impuestos" sheetId="6" r:id="rId8"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId9"/>
+  </externalReferences>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
@@ -23,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="102">
   <si>
     <t>Hosting</t>
   </si>
@@ -284,6 +288,51 @@
   </si>
   <si>
     <t>Asesoría Legal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asesoría legal </t>
+  </si>
+  <si>
+    <t>JUS</t>
+  </si>
+  <si>
+    <t>Calculo asesoría legal</t>
+  </si>
+  <si>
+    <t>Semestre 1 -2016</t>
+  </si>
+  <si>
+    <t>Semestre 2 -2016</t>
+  </si>
+  <si>
+    <t>Semestre 1 -2017</t>
+  </si>
+  <si>
+    <t>Semestre 2 -2017</t>
+  </si>
+  <si>
+    <t>Estandar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Premiun </t>
+  </si>
+  <si>
+    <t>Home semanal</t>
+  </si>
+  <si>
+    <t>Home mensual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-mail semanal </t>
+  </si>
+  <si>
+    <t>E-mail Mensual</t>
+  </si>
+  <si>
+    <t>Costo de asesoría legal=</t>
+  </si>
+  <si>
+    <t>Valor asesoría</t>
   </si>
 </sst>
 </file>
@@ -293,7 +342,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$$-2C0A]\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$$-2C0A]#,##0.00"/>
-    <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -319,7 +368,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -383,6 +432,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -453,7 +514,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -500,20 +561,26 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,6 +624,189 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="01-Tipo Ingreso"/>
+      <sheetName val="02-Volumenes Ingresos"/>
+      <sheetName val="03-Ingresos"/>
+      <sheetName val="04-Gastos"/>
+      <sheetName val="Ganancias"/>
+      <sheetName val="Indicadores Financieros"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="B3">
+            <v>10500</v>
+          </cell>
+          <cell r="C3">
+            <v>12810</v>
+          </cell>
+          <cell r="D3">
+            <v>15120</v>
+          </cell>
+          <cell r="E3">
+            <v>17430</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4">
+            <v>15000</v>
+          </cell>
+          <cell r="C4">
+            <v>18300</v>
+          </cell>
+          <cell r="D4">
+            <v>21600</v>
+          </cell>
+          <cell r="E4">
+            <v>24900</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6">
+            <v>1700</v>
+          </cell>
+          <cell r="C6">
+            <v>2074</v>
+          </cell>
+          <cell r="D6">
+            <v>2448</v>
+          </cell>
+          <cell r="E6">
+            <v>2822</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7">
+            <v>6500</v>
+          </cell>
+          <cell r="C7">
+            <v>7930</v>
+          </cell>
+          <cell r="D7">
+            <v>9360</v>
+          </cell>
+          <cell r="E7">
+            <v>10790</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8">
+            <v>500</v>
+          </cell>
+          <cell r="C8">
+            <v>610</v>
+          </cell>
+          <cell r="D8">
+            <v>720</v>
+          </cell>
+          <cell r="E8">
+            <v>830</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9">
+            <v>1400</v>
+          </cell>
+          <cell r="C9">
+            <v>1708</v>
+          </cell>
+          <cell r="D9">
+            <v>2016</v>
+          </cell>
+          <cell r="E9">
+            <v>2324</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="4">
+          <cell r="B4">
+            <v>13</v>
+          </cell>
+          <cell r="C4">
+            <v>2</v>
+          </cell>
+          <cell r="E4">
+            <v>4</v>
+          </cell>
+          <cell r="F4">
+            <v>4</v>
+          </cell>
+          <cell r="G4">
+            <v>5</v>
+          </cell>
+          <cell r="H4">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5">
+            <v>10</v>
+          </cell>
+          <cell r="C5">
+            <v>5</v>
+          </cell>
+          <cell r="E5">
+            <v>5</v>
+          </cell>
+          <cell r="H5">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6">
+            <v>13</v>
+          </cell>
+          <cell r="C6">
+            <v>7</v>
+          </cell>
+          <cell r="E6">
+            <v>6</v>
+          </cell>
+          <cell r="F6">
+            <v>5</v>
+          </cell>
+          <cell r="G6">
+            <v>5</v>
+          </cell>
+          <cell r="H6">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7">
+            <v>21</v>
+          </cell>
+          <cell r="C7">
+            <v>9</v>
+          </cell>
+          <cell r="E7">
+            <v>5</v>
+          </cell>
+          <cell r="F7">
+            <v>3</v>
+          </cell>
+          <cell r="G7">
+            <v>6</v>
+          </cell>
+          <cell r="H7">
+            <v>9</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1359,10 +1609,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S16"/>
+  <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1373,6 +1623,8 @@
     <col min="4" max="4" width="17.85546875" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -1397,8 +1649,12 @@
       <c r="G1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="H1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -1419,21 +1675,27 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="19"/>
-      <c r="G2" s="51">
+      <c r="G2" s="49">
         <v>0.2</v>
+      </c>
+      <c r="H2" s="49">
+        <v>0.03</v>
+      </c>
+      <c r="I2" s="56">
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46">
+      <c r="B3" s="44"/>
+      <c r="C3" s="44">
         <f>3980+3980*G2</f>
         <v>4776</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47">
+      <c r="D3" s="45"/>
+      <c r="E3" s="45">
         <f>3980+3980*60%</f>
         <v>6368</v>
       </c>
@@ -1443,23 +1705,23 @@
       <c r="A4" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="47">
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="45">
         <f>99500+99500*40%</f>
         <v>139300</v>
       </c>
-      <c r="E4" s="48"/>
+      <c r="E4" s="46"/>
       <c r="F4" s="20"/>
     </row>
     <row r="5" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="48"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="46"/>
       <c r="F5" s="20" t="s">
         <v>75</v>
       </c>
@@ -1468,19 +1730,19 @@
       <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="46">
+      <c r="B6" s="44">
         <f>('Estimacion de pedidos'!B4+'Estimacion de pedidos'!B4*'Estimacion de pedidos'!B11)*'Estimacion de pedidos'!B3*'Estimacion de pedidos'!B2*'Estimacion de pedidos'!B6</f>
         <v>73664.639999999999</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="44">
         <f>('Estimacion de pedidos'!B4+'Estimacion de pedidos'!B4*'Estimacion de pedidos'!B12)*'Estimacion de pedidos'!B3*'Estimacion de pedidos'!B2*'Estimacion de pedidos'!B6+B6*G2</f>
         <v>96582.528000000006</v>
       </c>
-      <c r="D6" s="47">
+      <c r="D6" s="45">
         <f>('Estimacion de pedidos'!B5+'Estimacion de pedidos'!B5*'Estimacion de pedidos'!B13)*'Estimacion de pedidos'!B3*'Estimacion de pedidos'!B2*'Estimacion de pedidos'!B6+C6*G2</f>
         <v>167055.0336</v>
       </c>
-      <c r="E6" s="48">
+      <c r="E6" s="46">
         <f>('Estimacion de pedidos'!B5+'Estimacion de pedidos'!B5*'Estimacion de pedidos'!B14)*'Estimacion de pedidos'!B3*'Estimacion de pedidos'!B2*'Estimacion de pedidos'!B6+D6*G2</f>
         <v>188925.24672</v>
       </c>
@@ -1490,19 +1752,19 @@
       <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="46">
+      <c r="B7" s="44">
         <f>C7+C7*'Estimacion de pedidos'!B11</f>
         <v>540</v>
       </c>
-      <c r="C7" s="46">
+      <c r="C7" s="44">
         <f>500+500*G2</f>
         <v>600</v>
       </c>
-      <c r="D7" s="47">
+      <c r="D7" s="45">
         <f>(C7+C7*'Estimacion de pedidos'!B13)+C7*G2</f>
         <v>690</v>
       </c>
-      <c r="E7" s="47">
+      <c r="E7" s="45">
         <f>(D7+D7*'Estimacion de pedidos'!B14)+D7*G2</f>
         <v>828</v>
       </c>
@@ -1512,19 +1774,19 @@
       <c r="A8" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="46">
+      <c r="B8" s="44">
         <f>SUM(B6:B7)</f>
         <v>74204.639999999999</v>
       </c>
-      <c r="C8" s="46">
+      <c r="C8" s="44">
         <f>SUM(C3:C7)</f>
         <v>101958.52800000001</v>
       </c>
-      <c r="D8" s="47">
+      <c r="D8" s="45">
         <f>SUM(D3:D7)</f>
         <v>307045.03359999997</v>
       </c>
-      <c r="E8" s="48">
+      <c r="E8" s="46">
         <f>SUM(E3:E7)</f>
         <v>196121.24672</v>
       </c>
@@ -1534,20 +1796,20 @@
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="50"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="48"/>
       <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="48"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="46"/>
       <c r="F10" s="20" t="s">
         <v>85</v>
       </c>
@@ -1556,53 +1818,74 @@
       <c r="A11" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
+      <c r="B11" s="44">
+        <f>'Costos legales'!H4</f>
+        <v>6264</v>
+      </c>
+      <c r="C11" s="44">
+        <f>'Costos legales'!H6</f>
+        <v>8300.880000000001</v>
+      </c>
+      <c r="D11" s="45">
+        <f>'Costos legales'!H8</f>
+        <v>12869.279999999999</v>
+      </c>
+      <c r="E11" s="45">
+        <f>'Costos legales'!H10</f>
+        <v>19875.18</v>
+      </c>
     </row>
     <row r="12" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="48"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="20"/>
     </row>
     <row r="13" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="50"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="48"/>
       <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="48"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="46"/>
       <c r="F14" s="20"/>
     </row>
     <row r="15" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="46"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="48"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="46"/>
       <c r="F15" s="20"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F16" s="22"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="43"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1611,6 +1894,307 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="59"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="61">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="59" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="43">
+        <f>'[1]02-Volumenes Ingresos'!$B$4*'[1]01-Tipo Ingreso'!$B$3</f>
+        <v>136500</v>
+      </c>
+      <c r="C3" s="43">
+        <f>'[1]02-Volumenes Ingresos'!$C$4*'[1]01-Tipo Ingreso'!$B$4</f>
+        <v>30000</v>
+      </c>
+      <c r="D3" s="43">
+        <f>'[1]02-Volumenes Ingresos'!$E$4*'[1]01-Tipo Ingreso'!$B$6</f>
+        <v>6800</v>
+      </c>
+      <c r="E3" s="43">
+        <f>'[1]02-Volumenes Ingresos'!$F$4*'[1]01-Tipo Ingreso'!$B$7</f>
+        <v>26000</v>
+      </c>
+      <c r="F3" s="43">
+        <f>'[1]02-Volumenes Ingresos'!$G$4*'[1]01-Tipo Ingreso'!$B$8</f>
+        <v>2500</v>
+      </c>
+      <c r="G3" s="43">
+        <f>'[1]02-Volumenes Ingresos'!$H$4*'[1]01-Tipo Ingreso'!$B$9</f>
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="58">
+        <f>B3*B1</f>
+        <v>4095</v>
+      </c>
+      <c r="C4" s="58">
+        <f>C3*B1</f>
+        <v>900</v>
+      </c>
+      <c r="D4" s="58">
+        <f>D3*B1</f>
+        <v>204</v>
+      </c>
+      <c r="E4" s="58">
+        <f>E3*B1</f>
+        <v>780</v>
+      </c>
+      <c r="F4" s="58">
+        <f>F3*B1</f>
+        <v>75</v>
+      </c>
+      <c r="G4" s="58">
+        <f>G3*B1</f>
+        <v>210</v>
+      </c>
+      <c r="H4" s="58">
+        <f>SUM(B4:G4)</f>
+        <v>6264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="43">
+        <f>'[1]02-Volumenes Ingresos'!$B$5*'[1]01-Tipo Ingreso'!$C$3</f>
+        <v>128100</v>
+      </c>
+      <c r="C5" s="43">
+        <f>'[1]02-Volumenes Ingresos'!$C$5*'[1]01-Tipo Ingreso'!$C$4</f>
+        <v>91500</v>
+      </c>
+      <c r="D5" s="43">
+        <f>'[1]02-Volumenes Ingresos'!$E$5*'[1]01-Tipo Ingreso'!$C$6</f>
+        <v>10370</v>
+      </c>
+      <c r="E5" s="43">
+        <f>'[1]02-Volumenes Ingresos'!$F$4*'[1]01-Tipo Ingreso'!$C$7</f>
+        <v>31720</v>
+      </c>
+      <c r="F5" s="43">
+        <f>'[1]02-Volumenes Ingresos'!$G$4*'[1]01-Tipo Ingreso'!$C$8</f>
+        <v>3050</v>
+      </c>
+      <c r="G5" s="43">
+        <f>'[1]02-Volumenes Ingresos'!$H$5*'[1]01-Tipo Ingreso'!$C$9</f>
+        <v>11956</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="58">
+        <f>B5*B1</f>
+        <v>3843</v>
+      </c>
+      <c r="C6" s="58">
+        <f>C5*B1</f>
+        <v>2745</v>
+      </c>
+      <c r="D6" s="58">
+        <f>D5*B1</f>
+        <v>311.09999999999997</v>
+      </c>
+      <c r="E6" s="58">
+        <f>E5*B1</f>
+        <v>951.59999999999991</v>
+      </c>
+      <c r="F6" s="58">
+        <f>F5*B1</f>
+        <v>91.5</v>
+      </c>
+      <c r="G6" s="58">
+        <f>G5*B1</f>
+        <v>358.68</v>
+      </c>
+      <c r="H6" s="58">
+        <f>SUM(B6:G6)</f>
+        <v>8300.880000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="43">
+        <f>'[1]02-Volumenes Ingresos'!$B$6*'[1]01-Tipo Ingreso'!$D$3</f>
+        <v>196560</v>
+      </c>
+      <c r="C7" s="43">
+        <f>'[1]02-Volumenes Ingresos'!$C$6*'[1]01-Tipo Ingreso'!$D$4</f>
+        <v>151200</v>
+      </c>
+      <c r="D7" s="43">
+        <f>'[1]02-Volumenes Ingresos'!$E$6*'[1]01-Tipo Ingreso'!$D$6</f>
+        <v>14688</v>
+      </c>
+      <c r="E7" s="43">
+        <f>'[1]02-Volumenes Ingresos'!$F$6*'[1]01-Tipo Ingreso'!$D$7</f>
+        <v>46800</v>
+      </c>
+      <c r="F7" s="43">
+        <f>'[1]02-Volumenes Ingresos'!$G$6*'[1]01-Tipo Ingreso'!$D$8</f>
+        <v>3600</v>
+      </c>
+      <c r="G7" s="43">
+        <f>'[1]02-Volumenes Ingresos'!$H$6*'[1]01-Tipo Ingreso'!$D$9</f>
+        <v>16128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="58">
+        <f>B7*B1</f>
+        <v>5896.8</v>
+      </c>
+      <c r="C8" s="58">
+        <f>C7*B1</f>
+        <v>4536</v>
+      </c>
+      <c r="D8" s="58">
+        <f>D7*B1</f>
+        <v>440.64</v>
+      </c>
+      <c r="E8" s="58">
+        <f>E7*B1</f>
+        <v>1404</v>
+      </c>
+      <c r="F8" s="58">
+        <f>F7*B1</f>
+        <v>108</v>
+      </c>
+      <c r="G8" s="58">
+        <f>G7*B1</f>
+        <v>483.84</v>
+      </c>
+      <c r="H8" s="58">
+        <f>SUM(B8:G8)</f>
+        <v>12869.279999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="43">
+        <f>'[1]02-Volumenes Ingresos'!$B$7*'[1]01-Tipo Ingreso'!$E$3</f>
+        <v>366030</v>
+      </c>
+      <c r="C9" s="43">
+        <f>'[1]02-Volumenes Ingresos'!$C$7*'[1]01-Tipo Ingreso'!$E$4</f>
+        <v>224100</v>
+      </c>
+      <c r="D9" s="43">
+        <f>'[1]02-Volumenes Ingresos'!$E$7*'[1]01-Tipo Ingreso'!$E$6</f>
+        <v>14110</v>
+      </c>
+      <c r="E9" s="43">
+        <f>'[1]02-Volumenes Ingresos'!$F$7*'[1]01-Tipo Ingreso'!$E$7</f>
+        <v>32370</v>
+      </c>
+      <c r="F9" s="43">
+        <f>'[1]02-Volumenes Ingresos'!$G$7*'[1]01-Tipo Ingreso'!$E$8</f>
+        <v>4980</v>
+      </c>
+      <c r="G9" s="43">
+        <f>'[1]02-Volumenes Ingresos'!$H$7*'[1]01-Tipo Ingreso'!$E$9</f>
+        <v>20916</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="58">
+        <f>B9*B1</f>
+        <v>10980.9</v>
+      </c>
+      <c r="C10" s="58">
+        <f>C9*B1</f>
+        <v>6723</v>
+      </c>
+      <c r="D10" s="58">
+        <f>D9*B1</f>
+        <v>423.3</v>
+      </c>
+      <c r="E10" s="58">
+        <f>E9*B1</f>
+        <v>971.09999999999991</v>
+      </c>
+      <c r="F10" s="58">
+        <f>F9*B1</f>
+        <v>149.4</v>
+      </c>
+      <c r="G10" s="58">
+        <f>G9*B1</f>
+        <v>627.48</v>
+      </c>
+      <c r="H10" s="58">
+        <f>SUM(B10:G10)</f>
+        <v>19875.18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -1625,16 +2209,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="53"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="53">
+      <c r="B2" s="50">
         <v>7</v>
       </c>
     </row>
@@ -1642,7 +2226,7 @@
       <c r="A3" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="53">
+      <c r="B3" s="50">
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
@@ -1650,7 +2234,7 @@
       <c r="A4" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="53">
+      <c r="B4" s="50">
         <v>25200</v>
       </c>
     </row>
@@ -1658,7 +2242,7 @@
       <c r="A5" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="53">
+      <c r="B5" s="50">
         <f>B4+B4*90%</f>
         <v>47880</v>
       </c>
@@ -1667,21 +2251,21 @@
       <c r="A6" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="54">
+      <c r="B6" s="51">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="52"/>
+      <c r="B9" s="53"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="50" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1689,7 +2273,7 @@
       <c r="A11" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="55">
+      <c r="B11" s="52">
         <v>-0.1</v>
       </c>
     </row>
@@ -1697,7 +2281,7 @@
       <c r="A12" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="55">
+      <c r="B12" s="52">
         <v>0</v>
       </c>
     </row>
@@ -1705,7 +2289,7 @@
       <c r="A13" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="55">
+      <c r="B13" s="52">
         <v>-0.05</v>
       </c>
     </row>
@@ -1713,7 +2297,7 @@
       <c r="A14" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="55">
+      <c r="B14" s="52">
         <v>0</v>
       </c>
     </row>
@@ -1726,7 +2310,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD28"/>
   <sheetViews>
@@ -2234,13 +2818,13 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="44" t="s">
+      <c r="A28" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2250,7 +2834,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
@@ -2411,7 +2995,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
@@ -2570,7 +3154,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>

</xml_diff>